<commit_message>
fixing template issue, creating digitization and processing tracking
</commit_message>
<xml_diff>
--- a/data/data_digitization/occurrence_data/1_raw_data/[collector_initials]-[journal_number]-occ-entry template.xlsx
+++ b/data/data_digitization/occurrence_data/1_raw_data/[collector_initials]-[journal_number]-occ-entry template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/data_digitization/occurrence_data/1_raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45BA867-FBD8-7146-B54D-AF33F58C6605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECAFE2C-7521-AF43-891F-293BE98514D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15340" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15440" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <author>Kyle Braak</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A8DDB6DB-164F-B542-BF28-66A88C3A6BAE}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{732410AC-6B8A-5248-AE77-A2B0B842646A}">
       <text>
         <r>
           <rPr>
@@ -129,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{C4C6551D-B61A-0F47-BF4B-625CAEB4EF97}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{11A953EE-CA77-6243-A02C-9C294653F884}">
       <text>
         <r>
           <rPr>
@@ -215,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{552BA6F0-B4A1-3441-A7FC-6A6D93AA887E}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{0607B1B7-AD65-A242-866D-BB8514ECBF49}">
       <text>
         <r>
           <rPr>
@@ -323,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{B42992FB-531D-9743-ADA0-2BD04AFE5FCA}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{4A57CE0F-C7AD-8648-8980-8A0AED1DD85B}">
       <text>
         <r>
           <rPr>
@@ -435,7 +435,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{C737CA67-21CB-4540-AEE9-D83B28E161DB}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{EB88FD54-CD0D-B441-B496-B95F4FC4D73F}">
       <text>
         <r>
           <rPr>
@@ -561,7 +561,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{274940BF-7D64-7141-8417-AC7302876D53}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{672A0EBE-9433-A94E-BED2-D955348ABF3F}">
       <text>
         <r>
           <rPr>
@@ -668,7 +668,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{DEAEAD63-48ED-2A4E-9FA0-F8A60DF75BFA}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{7B2C3724-E16F-4E44-BBEB-4623A744B7BD}">
       <text>
         <r>
           <rPr>
@@ -724,7 +724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{DC1234B4-128B-9D44-9647-ACD44B00D397}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{E5551A57-131E-2E4A-BE34-80094E93E54E}">
       <text>
         <r>
           <rPr>
@@ -850,7 +850,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{144860E7-37A9-7442-9661-FC5E9C626D31}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{91A5A8D8-F682-6D4D-B2DC-D0D01A848E3A}">
       <text>
         <r>
           <rPr>
@@ -936,7 +936,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{69A0DE11-3D9B-DD45-BD54-68EAC4E3B77F}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{EBD3CD19-9BFE-5B48-80F1-5C82A7D1F51C}">
       <text>
         <r>
           <rPr>
@@ -1022,7 +1022,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{FA07C549-45F1-6843-BD8A-5C29B980EF43}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{30FD4B1D-23D7-1145-B056-E0D6B319A5EB}">
       <text>
         <r>
           <rPr>
@@ -1108,7 +1108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{56E53AC6-F7E8-414E-9269-60273345448B}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{E18F86CF-8911-9A43-A42D-5E0F77F6539D}">
       <text>
         <r>
           <rPr>
@@ -1195,7 +1195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{0262923D-9B4C-7E48-B57E-DC6FA182E66C}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{C0FE8A6D-DEE3-0049-BB7C-C9A696C7AA56}">
       <text>
         <r>
           <rPr>
@@ -1281,7 +1281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{C09603FC-3352-834C-B4F5-F61FDEF58211}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{A2F25764-4BE8-0245-85D4-5F505ECE445E}">
       <text>
         <r>
           <rPr>
@@ -1348,7 +1348,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{CD0706FF-5811-BF49-993E-D0941F3AA07B}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{1762D171-209D-D947-8555-AFF34FF14DD2}">
       <text>
         <r>
           <rPr>
@@ -1434,7 +1434,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{83478F65-73DB-E043-B4E7-852EE638A389}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{C6473173-DDA5-D44D-87A7-A892FDDB11D3}">
       <text>
         <r>
           <rPr>
@@ -1507,7 +1507,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{D02977E1-488B-9F48-A6C9-AB421B4FC449}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{B9586400-66D1-7141-8F4F-DF928AA236E2}">
       <text>
         <r>
           <rPr>
@@ -1585,7 +1585,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{600D10A9-A6C8-C642-81F6-27CD7835EAC6}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{C334D07E-4730-1749-B76E-5A26B42DC1C1}">
       <text>
         <r>
           <rPr>
@@ -1682,7 +1682,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{31FD17C0-D5AE-6F41-8345-1A4EFE68544A}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{CA3A2C45-C583-DA43-877C-3A38B460B025}">
       <text>
         <r>
           <rPr>
@@ -1775,7 +1775,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="1" shapeId="0" xr:uid="{5B13E7B4-E6E7-D045-B018-8FAC95E81BC0}">
+    <comment ref="U1" authorId="1" shapeId="0" xr:uid="{9F8D95FB-54D3-F04C-9134-F2DD1CEAD6ED}">
       <text>
         <r>
           <rPr>
@@ -1871,7 +1871,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="1" shapeId="0" xr:uid="{B05819FB-05BF-4342-8D04-1FDAFB40A3C0}">
+    <comment ref="V1" authorId="1" shapeId="0" xr:uid="{A76DD89C-13AB-F048-A935-8FD1A912F16A}">
       <text>
         <r>
           <rPr>
@@ -1965,7 +1965,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{00D86AB6-65FF-F44F-B9EE-5D02C7CDA473}">
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{B3BFE285-5D7E-014B-96D5-A3177370E856}">
       <text>
         <r>
           <rPr>
@@ -2039,7 +2039,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{2410207F-8B4D-4246-9450-D9FC90711A12}">
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{C36EAF92-CB2B-8247-A6B4-E6839E892AD6}">
       <text>
         <r>
           <rPr>
@@ -2114,7 +2114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="1" shapeId="0" xr:uid="{2B56D7A6-70C4-964C-B53F-5099151A0A9C}">
+    <comment ref="Y1" authorId="1" shapeId="0" xr:uid="{4C5623D5-05B7-E844-824D-79860B5E2E43}">
       <text>
         <r>
           <rPr>
@@ -2189,7 +2189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{D0775F8C-E8A1-D240-B257-347544436168}">
+    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{02C4E6F9-C680-9A4E-8FE6-5FE3D6B276B0}">
       <text>
         <r>
           <rPr>
@@ -2263,7 +2263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{6547EF21-25AE-6F4F-AF2D-4DBC5EF0E9B5}">
+    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{1A1EB019-907B-974F-B8A9-28760AC102E7}">
       <text>
         <r>
           <rPr>
@@ -2338,7 +2338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{7FD26A50-5CA6-FE43-83AC-339CADE77507}">
+    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{44ACD083-7A9B-E146-B264-32980E3FE423}">
       <text>
         <r>
           <rPr>
@@ -2384,7 +2384,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{755321BC-C668-F042-8E31-CF64ED8C27AF}">
+    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{C09B578E-7BE1-1A44-890C-B5193E01F5A0}">
       <text>
         <r>
           <rPr>
@@ -2475,7 +2475,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>habitat</t>
   </si>
@@ -2540,9 +2540,6 @@
     <t>[vSciName]</t>
   </si>
   <si>
-    <t>[conf]</t>
-  </si>
-  <si>
     <t>[sciName]</t>
   </si>
   <si>
@@ -2561,83 +2558,26 @@
     <t>[island]</t>
   </si>
   <si>
-    <t>vCoordUncM</t>
+    <t>[conf]</t>
   </si>
   <si>
-    <t>British Columbia</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>Saturna Island</t>
-  </si>
-  <si>
-    <t>Ribes divaricatum (Common Gooseberry)</t>
-  </si>
-  <si>
-    <t>Ribes divaricatum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ribes divaricatum </t>
-  </si>
-  <si>
-    <t xml:space="preserve">m </t>
-  </si>
-  <si>
-    <t>Polystichum munitum (Sword fern)</t>
-  </si>
-  <si>
-    <t>Polystichum munitum</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>Salix scouleriana (scouler's pussy willow)</t>
-  </si>
-  <si>
-    <t>Salix scouleriana</t>
-  </si>
-  <si>
-    <t>Juniperus scopulorum</t>
-  </si>
-  <si>
-    <t>Juniperus scorpulorum</t>
-  </si>
-  <si>
-    <t>Collinsia parviflora</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grandiflora looks crossed out? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">collected up trail to Breezy Bay </t>
-  </si>
-  <si>
-    <t>idQualifier</t>
-  </si>
-  <si>
-    <t>Saturna Island; Taylor Point</t>
-  </si>
-  <si>
-    <t>Saturna Island; Breezy Bay; near bay</t>
+    <t>assColl</t>
   </si>
   <si>
     <t>assCollTaxa</t>
   </si>
   <si>
-    <t>assColl</t>
+    <t>vCoordUncM</t>
+  </si>
+  <si>
+    <t>idQualifier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2706,8 +2646,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2734,12 +2693,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE2F0DB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2EFDA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2772,7 +2725,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2783,13 +2736,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2797,6 +2755,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE2F0DB"/>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2809,7 +2773,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3097,7 +3061,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3105,103 +3069,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
-  <dimension ref="A1:AH64"/>
+  <dimension ref="A1:AF240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A271" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomLeft" activeCell="D276" sqref="D276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="6.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="24.83203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="7.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="24.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="3"/>
-    <col min="9" max="9" width="14.33203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="26" style="3" customWidth="1"/>
-    <col min="11" max="11" width="9" style="3" customWidth="1"/>
-    <col min="12" max="12" width="5.6640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="20.33203125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="19.1640625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="21.5" style="3" customWidth="1"/>
-    <col min="19" max="19" width="22.1640625" style="3" customWidth="1"/>
-    <col min="20" max="21" width="8.5" style="3" customWidth="1"/>
-    <col min="22" max="22" width="16.83203125" style="3" customWidth="1"/>
-    <col min="23" max="23" width="9.1640625" style="3" customWidth="1"/>
-    <col min="24" max="24" width="11.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="26" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9" style="3" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="3"/>
+    <col min="15" max="15" width="22.1640625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="29.5" style="3" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="11.83203125" style="3" customWidth="1"/>
+    <col min="20" max="20" width="8.5" style="3" customWidth="1"/>
+    <col min="21" max="21" width="9.1640625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="19.1640625" style="3" customWidth="1"/>
+    <col min="24" max="24" width="11.33203125" style="3" customWidth="1"/>
     <col min="25" max="25" width="7.5" style="3" customWidth="1"/>
     <col min="26" max="26" width="11.33203125" style="3" customWidth="1"/>
     <col min="27" max="27" width="11.1640625" style="3" customWidth="1"/>
     <col min="28" max="28" width="13" style="3" customWidth="1"/>
-    <col min="29" max="29" width="9.1640625" style="3" customWidth="1"/>
-    <col min="30" max="30" width="14.6640625" style="3" customWidth="1"/>
+    <col min="29" max="29" width="7.1640625" style="3" customWidth="1"/>
+    <col min="30" max="30" width="9" style="3" customWidth="1"/>
     <col min="31" max="31" width="10.83203125" style="3"/>
-    <col min="32" max="32" width="14.33203125" style="3" customWidth="1"/>
-    <col min="33" max="33" width="29.5" style="3" customWidth="1"/>
-    <col min="34" max="34" width="70.6640625" style="3" customWidth="1"/>
-    <col min="35" max="16384" width="10.83203125" style="3"/>
+    <col min="32" max="32" width="70.6640625" style="3" customWidth="1"/>
+    <col min="33" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="51" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>47</v>
+      <c r="L1" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>1</v>
@@ -3222,7 +3185,7 @@
         <v>8</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>12</v>
@@ -3249,261 +3212,110 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>10</v>
-      </c>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A2"/>
       <c r="B2"/>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1973039</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2"/>
+      <c r="F2" s="5"/>
       <c r="P2"/>
-      <c r="Q2"/>
-      <c r="AG2"/>
-      <c r="AH2"/>
-    </row>
-    <row r="3" spans="1:34" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>10</v>
-      </c>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="AF2"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A3"/>
       <c r="B3"/>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="3">
-        <v>19730311</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3"/>
-      <c r="P3"/>
-      <c r="Q3"/>
-      <c r="AH3"/>
-    </row>
-    <row r="4" spans="1:34" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>10</v>
-      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="AF3"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A4"/>
       <c r="B4"/>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="3">
-        <v>19730315</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4"/>
-    </row>
-    <row r="5" spans="1:34" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>11</v>
-      </c>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A5"/>
       <c r="B5"/>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="3">
-        <v>19730316</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5"/>
-      <c r="AH5"/>
-    </row>
-    <row r="6" spans="1:34" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>11</v>
-      </c>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="AF5"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A6"/>
       <c r="B6"/>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="3">
-        <v>19730316</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6"/>
-      <c r="AF6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH6"/>
-    </row>
-    <row r="7" spans="1:34" ht="68" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>11</v>
-      </c>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="AF6"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
       <c r="E7"/>
       <c r="F7"/>
-      <c r="G7" s="3">
-        <v>19730319</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="L7"/>
-      <c r="R7" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
-      <c r="L8"/>
-      <c r="AH8"/>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AF8"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
-      <c r="L9"/>
-      <c r="AH9"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AF9"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
-      <c r="L10"/>
-      <c r="AH10"/>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AF10"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
-      <c r="L11"/>
-      <c r="S11"/>
-      <c r="V11"/>
-      <c r="AH11"/>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="O11"/>
+      <c r="AF11"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12"/>
-      <c r="L12"/>
-      <c r="AH12"/>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AF12"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -3511,210 +3323,179 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="L13"/>
-      <c r="S13"/>
-      <c r="V13"/>
+      <c r="O13"/>
       <c r="AB13"/>
       <c r="AC13"/>
-      <c r="AH13"/>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AF13"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
-      <c r="L14"/>
-      <c r="S14"/>
-      <c r="V14"/>
-      <c r="AH14"/>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="O14"/>
+      <c r="AF14"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
-      <c r="L15"/>
-      <c r="S15"/>
-      <c r="V15"/>
-      <c r="AH15"/>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="O15"/>
+      <c r="AF15"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="L16"/>
-      <c r="S16"/>
-      <c r="V16"/>
-      <c r="AH16"/>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="O16"/>
+      <c r="AF16"/>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
-      <c r="L17"/>
-      <c r="S17"/>
-      <c r="V17"/>
-      <c r="AH17"/>
-    </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="O17"/>
+      <c r="AF17"/>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
-      <c r="L18"/>
-      <c r="S18"/>
-      <c r="V18"/>
-      <c r="AH18"/>
-    </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="O18"/>
+      <c r="AF18"/>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
-      <c r="L19"/>
-      <c r="S19"/>
-      <c r="V19"/>
-      <c r="AH19"/>
-    </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="O19"/>
+      <c r="AF19"/>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
-      <c r="L20"/>
-      <c r="S20"/>
-      <c r="V20"/>
-      <c r="AH20"/>
-    </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="O20"/>
+      <c r="AF20"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
-      <c r="L21"/>
-      <c r="S21"/>
-      <c r="V21"/>
-      <c r="AH21"/>
-    </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="O21"/>
+      <c r="AF21"/>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22"/>
-      <c r="L22"/>
-      <c r="S22"/>
-      <c r="V22"/>
-      <c r="AH22"/>
-    </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="O22"/>
+      <c r="AF22"/>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23"/>
-      <c r="L23"/>
-      <c r="S23"/>
-      <c r="V23"/>
-      <c r="AH23"/>
-    </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="O23"/>
+      <c r="AF23"/>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
-      <c r="L24"/>
-      <c r="S24"/>
-      <c r="V24"/>
-      <c r="AH24"/>
-    </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="O24"/>
+      <c r="AF24"/>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
-      <c r="L25"/>
-      <c r="S25"/>
-      <c r="V25"/>
-      <c r="AH25"/>
-    </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="O25"/>
+      <c r="AF25"/>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
-      <c r="L26"/>
-      <c r="S26"/>
-      <c r="V26"/>
-      <c r="AH26"/>
-    </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="O26"/>
+      <c r="AF26"/>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
-      <c r="L27"/>
-      <c r="V27"/>
-      <c r="AH27"/>
-    </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="R27"/>
+      <c r="AF27"/>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
-      <c r="L28"/>
-      <c r="AH28"/>
-    </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AF28"/>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
-      <c r="L29"/>
-      <c r="AH29"/>
-    </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AF29"/>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
-      <c r="L30"/>
-      <c r="AH30"/>
-    </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AF30"/>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
@@ -3722,261 +3503,271 @@
       <c r="E31"/>
       <c r="F31"/>
       <c r="L31"/>
-      <c r="AH31"/>
-    </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AB31"/>
+      <c r="AF31"/>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A32"/>
       <c r="B32"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33"/>
       <c r="B33"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34"/>
       <c r="B34"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35"/>
       <c r="B35"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36"/>
       <c r="B36"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37"/>
       <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-      <c r="L37"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
-      <c r="E38"/>
       <c r="F38"/>
-      <c r="L38"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39"/>
       <c r="B39"/>
-      <c r="C39"/>
       <c r="D39"/>
-      <c r="E39"/>
       <c r="F39"/>
-      <c r="L39"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
-      <c r="E40"/>
       <c r="F40"/>
-      <c r="L40"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
-      <c r="E41"/>
       <c r="F41"/>
-      <c r="L41"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
       <c r="D42"/>
-      <c r="E42"/>
       <c r="F42"/>
-      <c r="L42"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
       <c r="D43"/>
-      <c r="E43"/>
       <c r="F43"/>
-      <c r="L43"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
       <c r="D44"/>
-      <c r="E44"/>
       <c r="F44"/>
-      <c r="L44"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
       <c r="D45"/>
-      <c r="E45"/>
       <c r="F45"/>
-      <c r="L45"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
       <c r="D46"/>
-      <c r="E46"/>
       <c r="F46"/>
-      <c r="L46"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
       <c r="D47"/>
-      <c r="E47"/>
       <c r="F47"/>
-      <c r="L47"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
-      <c r="E48"/>
       <c r="F48"/>
-      <c r="L48"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49"/>
-      <c r="E49"/>
       <c r="F49"/>
-      <c r="L49"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50"/>
-      <c r="E50"/>
-      <c r="F50"/>
-      <c r="L50"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
-      <c r="E51"/>
       <c r="F51"/>
-      <c r="L51"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52"/>
-      <c r="E52"/>
       <c r="F52"/>
-      <c r="L52"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
       <c r="D53"/>
-      <c r="E53"/>
       <c r="F53"/>
-      <c r="L53"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54"/>
-      <c r="E54"/>
       <c r="F54"/>
-      <c r="L54"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55"/>
-      <c r="E55"/>
       <c r="F55"/>
-      <c r="L55"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56"/>
-      <c r="E56"/>
       <c r="F56"/>
-      <c r="L56"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L56" s="8"/>
+      <c r="AB56" s="8"/>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57"/>
-      <c r="E57"/>
       <c r="F57"/>
-      <c r="L57"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58"/>
-      <c r="E58"/>
       <c r="F58"/>
-      <c r="L58"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
       <c r="D59"/>
-      <c r="E59"/>
       <c r="F59"/>
-      <c r="L59"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
-      <c r="E60"/>
       <c r="F60"/>
-      <c r="L60"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
-      <c r="E61"/>
       <c r="F61"/>
-      <c r="L61"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A62"/>
       <c r="B62"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A63"/>
       <c r="B63"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B64"/>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B66"/>
+      <c r="L66" s="8"/>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B68"/>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B70"/>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B72"/>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B74"/>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B76"/>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B78"/>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B80"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B82"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B84"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B86"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B88"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B90"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B92"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B94"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B96"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B98"/>
+    </row>
+    <row r="120" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F120" s="9"/>
+    </row>
+    <row r="240" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D240" s="8"/>
+      <c r="F240" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>